<commit_message>
Floppy Interrupt, Floppy Maker (unity)
</commit_message>
<xml_diff>
--- a/Documentation/FloppyDisk.xlsx
+++ b/Documentation/FloppyDisk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24630" windowHeight="8820" xr2:uid="{4063F7FF-C7D8-46CE-BDB8-F783A7CEA58D}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24630" windowHeight="8820" xr2:uid="{4063F7FF-C7D8-46CE-BDB8-F783A7CEA58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TRACKS</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Get an interrupt when track is read?</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +503,7 @@
         <v>163840</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>

</xml_diff>